<commit_message>
Edits to LEDCON.BOM - added version info
</commit_message>
<xml_diff>
--- a/LEDCON.BOM.xlsx
+++ b/LEDCON.BOM.xlsx
@@ -11,12 +11,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="83">
   <si>
     <t>Product Name:</t>
   </si>
   <si>
-    <t>LED Controller</t>
+    <t>LED Controller (VER 1.1 REV B</t>
   </si>
   <si>
     <t>Tag:</t>
@@ -25,6 +25,9 @@
     <t>Product Number:</t>
   </si>
   <si>
+    <t>LEDCON</t>
+  </si>
+  <si>
     <t>Date:</t>
   </si>
   <si>
@@ -43,7 +46,7 @@
     <t>Drawing/Part No.</t>
   </si>
   <si>
-    <t>Tag</t>
+    <t>Version</t>
   </si>
   <si>
     <t>Date</t>
@@ -65,6 +68,9 @@
   </si>
   <si>
     <t>LEDCON.FACE</t>
+  </si>
+  <si>
+    <t>VER 1.0 REV A</t>
   </si>
   <si>
     <t>Mean Machine Inc.</t>
@@ -96,6 +102,9 @@
   </si>
   <si>
     <t>LEDCON.COREMID</t>
+  </si>
+  <si>
+    <t>VER 1.1 REV B</t>
   </si>
   <si>
     <t>Two Screw Core A</t>
@@ -490,7 +499,7 @@
     <col customWidth="1" min="3" max="3" width="31.14"/>
     <col customWidth="1" min="4" max="4" width="53.14"/>
     <col customWidth="1" min="5" max="5" width="30.43"/>
-    <col customWidth="1" min="6" max="6" width="15.0"/>
+    <col customWidth="1" min="6" max="6" width="18.57"/>
     <col customWidth="1" min="7" max="7" width="13.57"/>
     <col customWidth="1" min="8" max="8" width="38.86"/>
     <col customWidth="1" min="9" max="9" width="23.29"/>
@@ -532,10 +541,12 @@
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G2" s="7">
         <v>42010.0</v>
@@ -559,7 +570,7 @@
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
       <c r="F3" s="10" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G3" s="11">
         <v>42100.0</v>
@@ -578,32 +589,32 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="F4" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="G4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K4" s="4"/>
       <c r="L4" s="5"/>
@@ -680,18 +691,20 @@
       </c>
       <c r="B8" s="15"/>
       <c r="C8" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="13"/>
+        <v>18</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>19</v>
+      </c>
       <c r="G8" s="13"/>
       <c r="H8" s="15" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I8" s="15"/>
       <c r="J8" s="9"/>
@@ -730,13 +743,13 @@
       </c>
       <c r="B10" s="15"/>
       <c r="C10" s="15" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
@@ -758,18 +771,20 @@
       </c>
       <c r="B11" s="17"/>
       <c r="C11" s="15" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="13"/>
+        <v>26</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>19</v>
+      </c>
       <c r="G11" s="13"/>
       <c r="H11" s="15" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I11" s="15"/>
       <c r="J11" s="19"/>
@@ -788,18 +803,20 @@
       </c>
       <c r="B12" s="17"/>
       <c r="C12" s="15" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="13"/>
+        <v>29</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>30</v>
+      </c>
       <c r="G12" s="13"/>
       <c r="H12" s="15" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I12" s="15"/>
       <c r="J12" s="9"/>
@@ -818,18 +835,20 @@
       </c>
       <c r="B13" s="17"/>
       <c r="C13" s="15" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E13" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="13"/>
       <c r="G13" s="13"/>
       <c r="H13" s="15" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I13" s="13"/>
       <c r="J13" s="9"/>
@@ -848,18 +867,20 @@
       </c>
       <c r="B14" s="17"/>
       <c r="C14" s="15" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="13"/>
+        <v>36</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>30</v>
+      </c>
       <c r="G14" s="13"/>
       <c r="H14" s="15" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I14" s="13"/>
       <c r="J14" s="9"/>
@@ -878,18 +899,20 @@
       </c>
       <c r="B15" s="17"/>
       <c r="C15" s="15" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="F15" s="13"/>
+        <v>39</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>19</v>
+      </c>
       <c r="G15" s="13"/>
       <c r="H15" s="15" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I15" s="13"/>
       <c r="J15" s="9"/>
@@ -908,18 +931,18 @@
       </c>
       <c r="B16" s="17"/>
       <c r="C16" s="15" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
       <c r="H16" s="15" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="I16" s="13"/>
       <c r="J16" s="9"/>
@@ -958,21 +981,21 @@
       </c>
       <c r="B18" s="15"/>
       <c r="C18" s="15" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
       <c r="H18" s="15" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="I18" s="21" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="J18" s="9"/>
       <c r="K18" s="9"/>
@@ -1010,21 +1033,21 @@
       </c>
       <c r="B20" s="15"/>
       <c r="C20" s="15" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
       <c r="H20" s="15" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="I20" s="21" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
@@ -1062,21 +1085,21 @@
       </c>
       <c r="B22" s="15"/>
       <c r="C22" s="15" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F22" s="13"/>
       <c r="G22" s="13"/>
       <c r="H22" s="15" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="I22" s="21" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
@@ -1114,21 +1137,21 @@
       </c>
       <c r="B24" s="15"/>
       <c r="C24" s="15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="F24" s="13"/>
       <c r="G24" s="13"/>
       <c r="H24" s="24" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="I24" s="21" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="J24" s="9"/>
       <c r="K24" s="9"/>
@@ -1165,22 +1188,22 @@
         <v>2.0</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C26" s="12"/>
       <c r="D26" s="22" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E26" s="26" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F26" s="24"/>
       <c r="G26" s="12"/>
       <c r="H26" s="24" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="J26" s="24"/>
       <c r="K26" s="24"/>
@@ -1218,18 +1241,18 @@
       </c>
       <c r="B28" s="26"/>
       <c r="C28" s="29" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D28" s="28" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E28" s="28" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F28" s="24"/>
       <c r="G28" s="24"/>
       <c r="H28" s="28" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="I28" s="24"/>
       <c r="J28" s="24"/>
@@ -1267,22 +1290,22 @@
         <v>2.0</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C30" s="12"/>
       <c r="D30" s="22" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E30" s="26" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F30" s="24"/>
       <c r="G30" s="12"/>
       <c r="H30" s="24" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="I30" s="12" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="J30" s="24"/>
       <c r="K30" s="12"/>
@@ -1320,21 +1343,21 @@
       </c>
       <c r="B32" s="15"/>
       <c r="C32" s="15" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D32" s="30" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F32" s="13"/>
       <c r="G32" s="13"/>
       <c r="H32" s="15" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="I32" s="21" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
@@ -1372,21 +1395,21 @@
       </c>
       <c r="B34" s="15"/>
       <c r="C34" s="15" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D34" s="30" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F34" s="13"/>
       <c r="G34" s="13"/>
       <c r="H34" s="15" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="I34" s="21" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
@@ -1624,7 +1647,7 @@
       <c r="C46" s="13"/>
       <c r="D46" s="13"/>
       <c r="E46" s="13" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="F46" s="13"/>
       <c r="G46" s="13"/>

</xml_diff>